<commit_message>
Calculating pre moving average for one week reports prior five days
</commit_message>
<xml_diff>
--- a/moving average.xlsx
+++ b/moving average.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="true"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Moving Average" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Adjust Down" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="one_week_prior_five_days" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="42">
   <si>
     <t xml:space="preserve">Table 1</t>
   </si>
@@ -142,6 +143,12 @@
   <si>
     <t xml:space="preserve">EASTSIDE</t>
   </si>
+  <si>
+    <t xml:space="preserve">Pre Moving Average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standart Deviation</t>
+  </si>
 </sst>
 </file>
 
@@ -252,7 +259,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -361,6 +368,14 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -380,30 +395,30 @@
   </sheetPr>
   <dimension ref="A1:IV69"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K5" activeCellId="0" sqref="K5"/>
+      <selection pane="bottomRight" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.01020408163265"/>
-    <col collapsed="false" hidden="false" max="7" min="4" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="1" width="13.7959183673469"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="13.7959183673469"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="5.80612244897959"/>
+    <col collapsed="false" hidden="false" max="7" min="4" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="1" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="13.6326530612245"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="3.51020408163265"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="6.43367346938776"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="5.04081632653061"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="6.98469387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="7.40816326530612"/>
-    <col collapsed="false" hidden="false" max="256" min="19" style="1" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="6.3469387755102"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="4.86224489795918"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="256" min="19" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -674,35 +689,35 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="n">
         <f aca="true">TODAY()-7</f>
-        <v>41437</v>
+        <v>41521</v>
       </c>
       <c r="G2" s="4" t="n">
         <f aca="true">TODAY()-6</f>
-        <v>41438</v>
+        <v>41522</v>
       </c>
       <c r="H2" s="3" t="n">
         <f aca="true">TODAY()-5</f>
-        <v>41439</v>
+        <v>41523</v>
       </c>
       <c r="I2" s="3" t="n">
         <f aca="true">TODAY()-4</f>
-        <v>41440</v>
+        <v>41524</v>
       </c>
       <c r="J2" s="3" t="n">
         <f aca="true">TODAY()-3</f>
-        <v>41441</v>
+        <v>41525</v>
       </c>
       <c r="K2" s="3" t="n">
         <f aca="true">TODAY()-2</f>
-        <v>41442</v>
+        <v>41526</v>
       </c>
       <c r="L2" s="3" t="n">
         <f aca="true">TODAY()-1</f>
-        <v>41443</v>
+        <v>41527</v>
       </c>
       <c r="M2" s="3" t="n">
         <f aca="true">TODAY()</f>
-        <v>41444</v>
+        <v>41528</v>
       </c>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
@@ -1560,6 +1575,12 @@
       <c r="X5" s="8"/>
       <c r="Y5" s="8"/>
       <c r="Z5" s="8"/>
+      <c r="AA5" s="0"/>
+      <c r="AB5" s="0"/>
+      <c r="AC5" s="0"/>
+      <c r="AD5" s="0"/>
+      <c r="AE5" s="0"/>
+      <c r="AF5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="14"/>
@@ -1600,6 +1621,12 @@
       <c r="X6" s="8"/>
       <c r="Y6" s="8"/>
       <c r="Z6" s="8"/>
+      <c r="AA6" s="0"/>
+      <c r="AB6" s="0"/>
+      <c r="AC6" s="0"/>
+      <c r="AD6" s="0"/>
+      <c r="AE6" s="0"/>
+      <c r="AF6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="14"/>
@@ -1640,6 +1667,12 @@
       <c r="X7" s="8"/>
       <c r="Y7" s="8"/>
       <c r="Z7" s="8"/>
+      <c r="AA7" s="0"/>
+      <c r="AB7" s="0"/>
+      <c r="AC7" s="0"/>
+      <c r="AD7" s="0"/>
+      <c r="AE7" s="0"/>
+      <c r="AF7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="14"/>
@@ -1680,6 +1713,12 @@
       <c r="X8" s="8"/>
       <c r="Y8" s="8"/>
       <c r="Z8" s="8"/>
+      <c r="AA8" s="0"/>
+      <c r="AB8" s="0"/>
+      <c r="AC8" s="0"/>
+      <c r="AD8" s="0"/>
+      <c r="AE8" s="0"/>
+      <c r="AF8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14"/>
@@ -1714,6 +1753,12 @@
       <c r="X9" s="8"/>
       <c r="Y9" s="8"/>
       <c r="Z9" s="8"/>
+      <c r="AA9" s="0"/>
+      <c r="AB9" s="0"/>
+      <c r="AC9" s="0"/>
+      <c r="AD9" s="0"/>
+      <c r="AE9" s="0"/>
+      <c r="AF9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="14"/>
@@ -1742,6 +1787,12 @@
       <c r="X10" s="8"/>
       <c r="Y10" s="8"/>
       <c r="Z10" s="8"/>
+      <c r="AA10" s="0"/>
+      <c r="AB10" s="0"/>
+      <c r="AC10" s="0"/>
+      <c r="AD10" s="0"/>
+      <c r="AE10" s="0"/>
+      <c r="AF10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="14"/>
@@ -1770,6 +1821,12 @@
       <c r="X11" s="8"/>
       <c r="Y11" s="8"/>
       <c r="Z11" s="8"/>
+      <c r="AA11" s="0"/>
+      <c r="AB11" s="0"/>
+      <c r="AC11" s="0"/>
+      <c r="AD11" s="0"/>
+      <c r="AE11" s="0"/>
+      <c r="AF11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
@@ -1836,6 +1893,12 @@
       <c r="X12" s="8"/>
       <c r="Y12" s="8"/>
       <c r="Z12" s="8"/>
+      <c r="AA12" s="0"/>
+      <c r="AB12" s="0"/>
+      <c r="AC12" s="0"/>
+      <c r="AD12" s="0"/>
+      <c r="AE12" s="0"/>
+      <c r="AF12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="14"/>
@@ -1864,6 +1927,12 @@
       <c r="X13" s="8"/>
       <c r="Y13" s="8"/>
       <c r="Z13" s="8"/>
+      <c r="AA13" s="0"/>
+      <c r="AB13" s="0"/>
+      <c r="AC13" s="0"/>
+      <c r="AD13" s="0"/>
+      <c r="AE13" s="0"/>
+      <c r="AF13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
@@ -1929,6 +1998,12 @@
       <c r="X14" s="8"/>
       <c r="Y14" s="8"/>
       <c r="Z14" s="8"/>
+      <c r="AA14" s="0"/>
+      <c r="AB14" s="0"/>
+      <c r="AC14" s="0"/>
+      <c r="AD14" s="0"/>
+      <c r="AE14" s="0"/>
+      <c r="AF14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="20.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="15" t="s">
@@ -3366,11 +3441,11 @@
       </c>
       <c r="K45" s="8" t="n">
         <f aca="false">K44-J44</f>
-        <v>0.233333333333331</v>
+        <v>0.233333333333334</v>
       </c>
       <c r="L45" s="8" t="n">
         <f aca="false">L44-K44</f>
-        <v>5.26666666666667</v>
+        <v>5.26666666666666</v>
       </c>
       <c r="M45" s="8" t="n">
         <f aca="false">M44-L44</f>
@@ -4260,9 +4335,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="256" min="2" style="1" width="18.765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="256" min="2" style="1" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="1025" min="257" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4729,7 +4804,7 @@
       </c>
       <c r="J19" s="8" t="n">
         <f aca="false">J17-I17</f>
-        <v>3.09523809523809</v>
+        <v>3.0952380952381</v>
       </c>
       <c r="K19" s="8" t="n">
         <f aca="false">K17-J17</f>
@@ -5297,4 +5372,443 @@
     <oddFooter>&amp;C&amp;12&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:M14"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M16" activeCellId="0" sqref="M16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3" t="n">
+        <f aca="true">TODAY()-11</f>
+        <v>41517</v>
+      </c>
+      <c r="C1" s="4" t="n">
+        <f aca="true">TODAY()-10</f>
+        <v>41518</v>
+      </c>
+      <c r="D1" s="3" t="n">
+        <f aca="true">TODAY()-9</f>
+        <v>41519</v>
+      </c>
+      <c r="E1" s="4" t="n">
+        <f aca="true">TODAY()-8</f>
+        <v>41520</v>
+      </c>
+      <c r="F1" s="3" t="n">
+        <f aca="true">TODAY()-7</f>
+        <v>41521</v>
+      </c>
+      <c r="G1" s="4" t="n">
+        <f aca="true">TODAY()-6</f>
+        <v>41522</v>
+      </c>
+      <c r="H1" s="3" t="n">
+        <f aca="true">TODAY()-5</f>
+        <v>41523</v>
+      </c>
+      <c r="I1" s="3" t="n">
+        <f aca="true">TODAY()-4</f>
+        <v>41524</v>
+      </c>
+      <c r="J1" s="3" t="n">
+        <f aca="true">TODAY()-3</f>
+        <v>41525</v>
+      </c>
+      <c r="K1" s="3" t="n">
+        <f aca="true">TODAY()-2</f>
+        <v>41526</v>
+      </c>
+      <c r="L1" s="3" t="n">
+        <f aca="true">TODAY()-1</f>
+        <v>41527</v>
+      </c>
+      <c r="M1" s="3" t="n">
+        <f aca="true">TODAY()</f>
+        <v>41528</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="18.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8" t="n">
+        <v>8</v>
+      </c>
+      <c r="G2" s="8" t="n">
+        <v>7</v>
+      </c>
+      <c r="H2" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="I2" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="J2" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="K2" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="L2" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="M2" s="8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M3" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="14"/>
+      <c r="B4" s="8" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="C4" s="8" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D4" s="8" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E4" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="L4" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="M4" s="8" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="14"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="K5" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="L5" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="M5" s="8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="14"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="K6" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="M6" s="8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="14"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="M7" s="8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="L8" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="M8" s="8" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="14"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="14"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="8" t="n">
+        <f aca="false">AVERAGE(B4:B10)</f>
+        <v>0.75</v>
+      </c>
+      <c r="C11" s="8" t="n">
+        <f aca="false">AVERAGE(C4:C10)</f>
+        <v>0.8</v>
+      </c>
+      <c r="D11" s="8" t="n">
+        <f aca="false">AVERAGE(D4:D10)</f>
+        <v>0.9</v>
+      </c>
+      <c r="E11" s="8" t="n">
+        <f aca="false">AVERAGE(E4:E10)</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="8" t="n">
+        <f aca="false">AVERAGE(F4:F10)</f>
+        <v>1</v>
+      </c>
+      <c r="G11" s="11" t="n">
+        <f aca="false">AVERAGE(G4:G10)</f>
+        <v>1.5</v>
+      </c>
+      <c r="H11" s="8" t="n">
+        <f aca="false">AVERAGE(H4:H10)</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="8" t="n">
+        <f aca="false">AVERAGE(I4:I10)</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="8" t="n">
+        <f aca="false">AVERAGE(J4:J10)</f>
+        <v>1.75</v>
+      </c>
+      <c r="K11" s="8" t="n">
+        <f aca="false">AVERAGE(K4:K10)</f>
+        <v>1.8</v>
+      </c>
+      <c r="L11" s="8" t="n">
+        <f aca="false">AVERAGE(L4:L10)</f>
+        <v>3.2</v>
+      </c>
+      <c r="M11" s="8" t="n">
+        <f aca="false">AVERAGE(M4:M10)</f>
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="28" t="n">
+        <f aca="false">AVERAGE(G11:M11)</f>
+        <v>1.66428571428571</v>
+      </c>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+    </row>
+    <row r="13" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="28" t="n">
+        <f aca="false">AVERAGE(B11:H11)</f>
+        <v>0.85</v>
+      </c>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+    </row>
+    <row r="14" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="28" t="n">
+        <f aca="false">G12-B13</f>
+        <v>0.814285714285714</v>
+      </c>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="G12:M12"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B14:M14"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>